<commit_message>
Design Doc v1.2 updated
Updated as per the discussions on 11-12 Nov at Delhi
</commit_message>
<xml_diff>
--- a/DataDictionary_GrevolVCU.xlsx
+++ b/DataDictionary_GrevolVCU.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Grevol\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Grevol\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAA67F0-6A1E-40A5-BCC6-10DC593DA342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88766A5A-B27D-43FF-9DD3-3737ADEC13F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="248">
   <si>
     <t>UC Pin</t>
   </si>
@@ -505,12 +505,6 @@
   </si>
   <si>
     <t>At ignition ON and previous check done &gt; x hours, if leakage HL and leakage LL diff &gt; xV</t>
-  </si>
-  <si>
-    <t>Open the contactor and close back after ignition cycle</t>
-  </si>
-  <si>
-    <t>If contactor logically turned ON and Vls not equal to Vbs OR contactor is logically OFF and Vls &gt; 10V</t>
   </si>
   <si>
     <t>Allow driving in limp home mode when driving possible</t>
@@ -673,9 +667,6 @@
     <t>*checkum for memory check at interval</t>
   </si>
   <si>
-    <t>Telematics comm fault</t>
-  </si>
-  <si>
     <t>*black box data to be staored in s-flash - includeing fault and data dump</t>
   </si>
   <si>
@@ -704,6 +695,97 @@
   </si>
   <si>
     <t>Open the contactor and shutdown the system</t>
+  </si>
+  <si>
+    <t>3 levels of thresholds for UV</t>
+  </si>
+  <si>
+    <t>Regen contrtol based on voltage little lower threshold</t>
+  </si>
+  <si>
+    <t>Open the contactor for 1 sec - allow opening within a band</t>
+  </si>
+  <si>
+    <t>If chargng is detected during ignition ON</t>
+  </si>
+  <si>
+    <t>Battery Enclosure Breach Fault</t>
+  </si>
+  <si>
+    <t>Battery Enclosure is Opened</t>
+  </si>
+  <si>
+    <t>Pack completely shutdown and send SMS Alert for battery breach</t>
+  </si>
+  <si>
+    <t>Pack needs to be brought to factory and cannot be restrt through server</t>
+  </si>
+  <si>
+    <t>No communication between Iot and BMS</t>
+  </si>
+  <si>
+    <t>Battery to be shutdown after 30 mins and SMS sent to server</t>
+  </si>
+  <si>
+    <t>Battery pack turned back ON through server comand once communication is established</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery to be shutdown after 5 mins </t>
+  </si>
+  <si>
+    <t>IOT_VCU comm fault</t>
+  </si>
+  <si>
+    <t>IOT_SERVER comm fault</t>
+  </si>
+  <si>
+    <t>No communication between IOT and server</t>
+  </si>
+  <si>
+    <t>Battery to be shutdown after lease stop date</t>
+  </si>
+  <si>
+    <t>Wiring fault</t>
+  </si>
+  <si>
+    <t>Significant difference between cell v sum and the total battery pack voltage</t>
+  </si>
+  <si>
+    <t>If SOC &gt; 10 and &lt; 90, go to limp home mode for 5 mins and then open the contactor. Limit the Ah extracted form the battery pack as safety</t>
+  </si>
+  <si>
+    <t>Vehicle to be broughtfor service for contactor replacement</t>
+  </si>
+  <si>
+    <t>If contactor logically turned ON and Vls not equal to Vbs OR contactor is logically OFF and Vls &gt; 10V
+If significant spikes are seen in the difference between voltage before contactor and voltage after contactor - 7kHz HPF for detection</t>
+  </si>
+  <si>
+    <t>Gear Slip fault</t>
+  </si>
+  <si>
+    <t>If the ratio of gearbox output shaft speed and motor RPM is outside of an expected range</t>
+  </si>
+  <si>
+    <t>Vehicle to be set to limp home mode and capacity limited so that the vehicle can be brought for servicing</t>
+  </si>
+  <si>
+    <t>Open the positive line contactor and the negative line relay and close back after ignition cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If motor controller max temperature rate of rise per unit of power is more than a certain limit </t>
+  </si>
+  <si>
+    <t>Motor Controller Hot warning</t>
+  </si>
+  <si>
+    <t>Heat sink effectiveness loss due to mud layer</t>
+  </si>
+  <si>
+    <t>Motor hot warning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If motor  max temperature rate of rise per unit of phase current square is more than a certain limit </t>
   </si>
 </sst>
 </file>
@@ -882,7 +964,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -938,6 +1020,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1761,10 +1852,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4978D81E-6A6B-48BE-B457-437087244080}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,12 +1893,14 @@
         <v>105</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="D3" s="12"/>
+        <v>190</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
@@ -1820,16 +1913,16 @@
         <v>139</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G4" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="H4" s="18" t="s">
         <v>200</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1842,9 +1935,11 @@
       <c r="C5" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="12" t="s">
+        <v>218</v>
+      </c>
       <c r="F5" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1855,11 +1950,11 @@
         <v>141</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D6" s="12"/>
       <c r="F6" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1874,7 +1969,7 @@
       </c>
       <c r="D7" s="12"/>
       <c r="F7" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1888,10 +1983,10 @@
         <v>139</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1902,13 +1997,13 @@
         <v>145</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>139</v>
+        <v>220</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1916,16 +2011,16 @@
         <v>112</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>147</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1936,30 +2031,30 @@
         <v>146</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>147</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>114</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>150</v>
+        <v>236</v>
       </c>
       <c r="D12" s="12" t="s">
         <v>151</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1974,7 +2069,7 @@
       </c>
       <c r="D13" s="12"/>
       <c r="F13" s="13" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1982,10 +2077,10 @@
         <v>116</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D14" s="12"/>
     </row>
@@ -1999,7 +2094,9 @@
       <c r="C15" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
@@ -2009,7 +2106,7 @@
         <v>154</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>155</v>
+        <v>242</v>
       </c>
       <c r="D16" s="12"/>
     </row>
@@ -2018,24 +2115,26 @@
         <v>124</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
     </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>119</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>156</v>
+        <v>238</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="D18" s="12"/>
+        <v>155</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>237</v>
+      </c>
       <c r="E18" s="15" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2043,7 +2142,7 @@
         <v>120</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
@@ -2053,14 +2152,14 @@
         <v>121</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -2068,7 +2167,7 @@
         <v>122</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
@@ -2078,86 +2177,86 @@
         <v>123</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D22" s="12"/>
     </row>
     <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>161</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>163</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="15" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>165</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>167</v>
       </c>
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="1:5" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
     </row>
     <row r="27" spans="1:5" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -2165,168 +2264,254 @@
     </row>
     <row r="30" spans="1:5" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="B30" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>220</v>
-      </c>
       <c r="D30" s="12"/>
     </row>
-    <row r="31" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
+    <row r="31" spans="1:5" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D32" s="12"/>
+    </row>
+    <row r="33" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B36" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C36" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D36" s="17" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-    </row>
-    <row r="37" spans="1:4" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>171</v>
-      </c>
+    <row r="37" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
     </row>
     <row r="38" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
     </row>
-    <row r="39" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>191</v>
+        <v>126</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
     </row>
     <row r="40" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
     </row>
-    <row r="41" spans="1:4" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>173</v>
+        <v>128</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>189</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11"/>
     </row>
-    <row r="42" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C42" s="11"/>
+        <v>170</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>229</v>
+      </c>
       <c r="D42" s="11"/>
     </row>
-    <row r="43" spans="1:4" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
-        <v>189</v>
+    <row r="43" spans="1:4" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>130</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
-        <v>177</v>
+        <v>131</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
+    <row r="45" spans="1:4" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
+        <v>175</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>227</v>
+      </c>
+      <c r="D48" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>233</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="D50" s="10"/>
+    </row>
+    <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>244</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="D52" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A35:D35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>